<commit_message>
main - add diagrama
</commit_message>
<xml_diff>
--- a/trabalho3_1/display_sete_seg.xlsx
+++ b/trabalho3_1/display_sete_seg.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\cl\trabalho3_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Downloads\trabalho3_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B62E350-1244-46E0-B66C-D5475EDEB15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48604D28-F0C7-4290-A6EA-ED3E68B7CD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48D17250-51EA-4470-9425-9C0AB866C90C}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{48D17250-51EA-4470-9425-9C0AB866C90C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>a</t>
   </si>
@@ -85,48 +83,12 @@
     <t>1010</t>
   </si>
   <si>
-    <t>hexa</t>
-  </si>
-  <si>
-    <t>bina</t>
-  </si>
-  <si>
     <t>out</t>
   </si>
   <si>
     <t>0110000</t>
   </si>
   <si>
-    <t>1111110</t>
-  </si>
-  <si>
-    <t>1101101</t>
-  </si>
-  <si>
-    <t>1111001</t>
-  </si>
-  <si>
-    <t>1011011</t>
-  </si>
-  <si>
-    <t>1011111</t>
-  </si>
-  <si>
-    <t>1110000</t>
-  </si>
-  <si>
-    <t>1111111</t>
-  </si>
-  <si>
-    <t>1111011</t>
-  </si>
-  <si>
-    <t>1110111</t>
-  </si>
-  <si>
-    <t>0011111</t>
-  </si>
-  <si>
     <t>1011</t>
   </si>
   <si>
@@ -145,19 +107,106 @@
     <t>0110</t>
   </si>
   <si>
-    <t>1001110</t>
-  </si>
-  <si>
     <t>1001111</t>
   </si>
   <si>
-    <t>1000111</t>
-  </si>
-  <si>
-    <t>0110011</t>
-  </si>
-  <si>
-    <t>0111101</t>
+    <t>0000001</t>
+  </si>
+  <si>
+    <t>0010010</t>
+  </si>
+  <si>
+    <t>0000110</t>
+  </si>
+  <si>
+    <t>1001100</t>
+  </si>
+  <si>
+    <t>0100100</t>
+  </si>
+  <si>
+    <t>0100000</t>
+  </si>
+  <si>
+    <t>0001111</t>
+  </si>
+  <si>
+    <t>0000000</t>
+  </si>
+  <si>
+    <t>0000100</t>
+  </si>
+  <si>
+    <t>0001000</t>
+  </si>
+  <si>
+    <t>1100000</t>
+  </si>
+  <si>
+    <t>0110001</t>
+  </si>
+  <si>
+    <t>1000010</t>
+  </si>
+  <si>
+    <t>0111000</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>hexadecimal</t>
+  </si>
+  <si>
+    <t>in (binario)</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -223,7 +272,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -522,166 +571,210 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
     <col min="5" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="9.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>36</v>
@@ -689,32 +782,41 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>38</v>

</xml_diff>